<commit_message>
finished connecting UI w/ script
</commit_message>
<xml_diff>
--- a/ExcelDogovor/lists/IT_project.xlsx
+++ b/ExcelDogovor/lists/IT_project.xlsx
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="111" uniqueCount="57">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="113" uniqueCount="59">
   <si>
     <t>GROUP_NAME:</t>
   </si>
@@ -55,9 +55,6 @@
     <t>PROJECT</t>
   </si>
   <si>
-    <t>"EXAMPLE"</t>
-  </si>
-  <si>
     <t>Artem Osincev</t>
   </si>
   <si>
@@ -157,12 +154,6 @@
     <t>STUD_Serial</t>
   </si>
   <si>
-    <t>PAR_Serial</t>
-  </si>
-  <si>
-    <t>PAR_Num</t>
-  </si>
-  <si>
     <t>STUD_Num</t>
   </si>
   <si>
@@ -184,13 +175,28 @@
     <t>УФМС по Кировскому району</t>
   </si>
   <si>
-    <t>УФМС по Советскому району</t>
-  </si>
-  <si>
     <t>LIVING_ADRESS:</t>
   </si>
   <si>
     <t>ул. Учебная, 228, кв. 63</t>
+  </si>
+  <si>
+    <t>03.09.2019</t>
+  </si>
+  <si>
+    <t>30.12.2019</t>
+  </si>
+  <si>
+    <t>«Информационные технологии: от «умного» чайника до автоматизированного производства»</t>
+  </si>
+  <si>
+    <t>777777</t>
+  </si>
+  <si>
+    <t>77 77</t>
+  </si>
+  <si>
+    <t>отделом УФМС России по Томской области в кировском районе г.Томска</t>
   </si>
   <si>
     <t>SEX:</t>
@@ -203,6 +209,9 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <numFmts count="1">
+    <numFmt numFmtId="164" formatCode="[$-F800]dddd\,\ mmmm\ dd\,\ yyyy"/>
+  </numFmts>
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -232,7 +241,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="right"/>
@@ -243,13 +252,14 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Обычный" xfId="0" builtinId="0"/>
@@ -533,7 +543,7 @@
   <dimension ref="A1:B12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A12" sqref="A12"/>
+      <selection activeCell="E7" sqref="E7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -554,7 +564,7 @@
         <v>0</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>9</v>
+        <v>53</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
@@ -578,7 +588,7 @@
         <v>2</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
@@ -599,23 +609,23 @@
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>48</v>
-      </c>
-      <c r="B10" s="6">
-        <v>43711</v>
+        <v>45</v>
+      </c>
+      <c r="B10" s="5" t="s">
+        <v>51</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>49</v>
-      </c>
-      <c r="B11" s="6">
-        <v>43829</v>
+        <v>46</v>
+      </c>
+      <c r="B11" s="5" t="s">
+        <v>52</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="B12">
         <v>18</v>
@@ -623,6 +633,7 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -642,22 +653,22 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C4">
         <f ca="1">DATEDIF(B4,TODAY(),"Y")</f>
@@ -666,47 +677,47 @@
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" s="3" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" s="3" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" s="3" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" s="3" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" s="3" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10" s="3" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11" s="3" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A12" s="3" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A13" s="3" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.25">
@@ -726,22 +737,22 @@
     </row>
     <row r="18" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A18" s="3" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="19" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A19" s="3" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="20" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A20" s="3" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="21" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A21" s="3" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
   </sheetData>
@@ -768,7 +779,7 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B1" s="3">
         <v>777777</v>
@@ -776,45 +787,46 @@
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C2" s="1"/>
       <c r="D2" s="1"/>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="B4" s="4">
+        <v>13</v>
+      </c>
+      <c r="B4" s="7">
         <v>37772</v>
       </c>
-      <c r="C4" s="5">
+      <c r="C4" s="4">
         <f ca="1">DATEDIF(B4,TODAY(),"Y")</f>
         <v>16</v>
       </c>
+      <c r="D4" s="6"/>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" s="3" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" s="3" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B6" s="3">
         <v>1</v>
@@ -822,120 +834,121 @@
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" s="3" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" s="3" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" s="3" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B9" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="C9" t="s">
         <v>42</v>
-      </c>
-      <c r="C9" t="s">
-        <v>45</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" s="3" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B10" s="3" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" s="3" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B11" s="3" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" s="3" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B12" s="3" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13" s="3" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B13" s="3" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14" s="3" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B14" s="3" t="s">
-        <v>43</v>
-      </c>
-      <c r="C14" t="s">
-        <v>44</v>
+        <v>55</v>
+      </c>
+      <c r="C14" s="5" t="s">
+        <v>54</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A15" s="3" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B15" s="3" t="s">
-        <v>52</v>
+        <v>56</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A16" s="3" t="s">
-        <v>53</v>
+        <v>49</v>
       </c>
       <c r="B16" s="3" t="s">
-        <v>54</v>
+        <v>50</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A17" s="3" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="B17" s="3" t="s">
-        <v>56</v>
+        <v>58</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A20" s="3" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A21" s="3" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A22" s="3" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A23" s="3" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -955,22 +968,22 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C4">
         <f ca="1">DATEDIF(B4,TODAY(),"Y")</f>
@@ -979,47 +992,47 @@
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" s="3" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" s="3" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" s="3" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" s="3" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" s="3" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10" s="3" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11" s="3" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A12" s="3" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A13" s="3" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.25">
@@ -1039,22 +1052,22 @@
     </row>
     <row r="18" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A18" s="3" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="19" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A19" s="3" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="20" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A20" s="3" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="21" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A21" s="3" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
   </sheetData>
@@ -1078,22 +1091,22 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C4">
         <f ca="1">DATEDIF(B4,TODAY(),"Y")</f>
@@ -1102,47 +1115,47 @@
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" s="3" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" s="3" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" s="3" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" s="3" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" s="3" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10" s="3" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11" s="3" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A12" s="3" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A13" s="3" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.25">
@@ -1162,22 +1175,22 @@
     </row>
     <row r="18" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A18" s="3" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="19" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A19" s="3" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="20" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A20" s="3" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="21" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A21" s="3" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
   </sheetData>

</xml_diff>